<commit_message>
Agrego contenido de variables estacionalizadas
</commit_message>
<xml_diff>
--- a/Series-de-Tiempo/datos/emae.xlsx
+++ b/Series-de-Tiempo/datos/emae.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D188"/>
+  <dimension ref="A1:D189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,10 +417,10 @@
         <v>92.62750602691051</v>
       </c>
       <c r="C2">
-        <v>98.44847585457256</v>
+        <v>98.44644059187507</v>
       </c>
       <c r="D2">
-        <v>96.04433627895963</v>
+        <v>96.0458100922521</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -431,10 +431,10 @@
         <v>90.1861793165596</v>
       </c>
       <c r="C3">
-        <v>98.28904328240463</v>
+        <v>98.2859192068772</v>
       </c>
       <c r="D3">
-        <v>96.64369707758156</v>
+        <v>96.64495644580296</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -445,10 +445,10 @@
         <v>101.8832980423807</v>
       </c>
       <c r="C4">
-        <v>97.4860716077727</v>
+        <v>97.49123094599938</v>
       </c>
       <c r="D4">
-        <v>97.30612805728364</v>
+        <v>97.3071896768643</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -459,10 +459,10 @@
         <v>102.5674302511826</v>
       </c>
       <c r="C5">
-        <v>95.53365332974144</v>
+        <v>95.53050576885636</v>
       </c>
       <c r="D5">
-        <v>97.99830718001093</v>
+        <v>97.9990208617124</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -473,10 +473,10 @@
         <v>109.8775039405166</v>
       </c>
       <c r="C6">
-        <v>96.65664898237415</v>
+        <v>96.65817796022664</v>
       </c>
       <c r="D6">
-        <v>98.71943243895626</v>
+        <v>98.71985343261602</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -487,10 +487,10 @@
         <v>105.6624062020985</v>
       </c>
       <c r="C7">
-        <v>98.45237216447451</v>
+        <v>98.45399074750787</v>
       </c>
       <c r="D7">
-        <v>99.46460251772942</v>
+        <v>99.46469027588391</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -501,10 +501,10 @@
         <v>101.1069972900212</v>
       </c>
       <c r="C8">
-        <v>100.9556662036567</v>
+        <v>100.9556580216852</v>
       </c>
       <c r="D8">
-        <v>100.2383221799637</v>
+        <v>100.2380639967311</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -515,10 +515,10 @@
         <v>98.35573694243756</v>
       </c>
       <c r="C9">
-        <v>101.9278768779535</v>
+        <v>101.9274973074355</v>
       </c>
       <c r="D9">
-        <v>101.0423920427755</v>
+        <v>101.0417828931555</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -529,10 +529,10 @@
         <v>98.08637453469638</v>
       </c>
       <c r="C10">
-        <v>102.4704760787243</v>
+        <v>102.4708638312134</v>
       </c>
       <c r="D10">
-        <v>101.8716523979185</v>
+        <v>101.8707611571919</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -543,10 +543,10 @@
         <v>97.8356659809799</v>
       </c>
       <c r="C11">
-        <v>103.2236052669281</v>
+        <v>103.222782895258</v>
       </c>
       <c r="D11">
-        <v>102.7185429453871</v>
+        <v>102.7174784441498</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -557,10 +557,10 @@
         <v>100.1319466812214</v>
       </c>
       <c r="C12">
-        <v>103.000197191927</v>
+        <v>102.9988532041698</v>
       </c>
       <c r="D12">
-        <v>103.563778426712</v>
+        <v>103.5626629863908</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -571,10 +571,10 @@
         <v>101.6789547909953</v>
       </c>
       <c r="C13">
-        <v>103.5559131594704</v>
+        <v>103.5580795188957</v>
       </c>
       <c r="D13">
-        <v>104.3888084567219</v>
+        <v>104.387729737249</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -585,10 +585,10 @@
         <v>98.47335952917901</v>
       </c>
       <c r="C14">
-        <v>105.5403112802187</v>
+        <v>105.539246479818</v>
       </c>
       <c r="D14">
-        <v>105.1777422943122</v>
+        <v>105.1767793850112</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -599,10 +599,10 @@
         <v>96.11886613343405</v>
       </c>
       <c r="C15">
-        <v>106.1065957188219</v>
+        <v>106.1030707521411</v>
       </c>
       <c r="D15">
-        <v>105.9192113258046</v>
+        <v>105.9184387220898</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -613,10 +613,10 @@
         <v>110.6564258671952</v>
       </c>
       <c r="C16">
-        <v>107.1101386972952</v>
+        <v>107.1147284643737</v>
       </c>
       <c r="D16">
-        <v>106.6102694411697</v>
+        <v>106.6097435078768</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -627,10 +627,10 @@
         <v>116.5451904821491</v>
       </c>
       <c r="C17">
-        <v>108.1062429041448</v>
+        <v>108.1026028389259</v>
       </c>
       <c r="D17">
-        <v>107.2549077722094</v>
+        <v>107.2546407098749</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -641,10 +641,10 @@
         <v>126.6619433550273</v>
       </c>
       <c r="C18">
-        <v>108.8700638862761</v>
+        <v>108.8712513476743</v>
       </c>
       <c r="D18">
-        <v>107.8629030783158</v>
+        <v>107.8629365652748</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -655,10 +655,10 @@
         <v>116.5022232149288</v>
       </c>
       <c r="C19">
-        <v>108.5588783107902</v>
+        <v>108.5613309146066</v>
       </c>
       <c r="D19">
-        <v>108.4497876168488</v>
+        <v>108.4501310602309</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -669,10 +669,10 @@
         <v>107.5811392624596</v>
       </c>
       <c r="C20">
-        <v>109.2305652667161</v>
+        <v>109.2305121232816</v>
       </c>
       <c r="D20">
-        <v>109.0333963888928</v>
+        <v>109.0340095721231</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -683,10 +683,10 @@
         <v>105.8208927931011</v>
       </c>
       <c r="C21">
-        <v>109.3744256094638</v>
+        <v>109.3741613008765</v>
       </c>
       <c r="D21">
-        <v>109.6304709540061</v>
+        <v>109.6312582282728</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -697,10 +697,10 @@
         <v>104.8921347267232</v>
       </c>
       <c r="C22">
-        <v>109.1371040965169</v>
+        <v>109.1374215485336</v>
       </c>
       <c r="D22">
-        <v>110.2535012387146</v>
+        <v>110.2543316555141</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -711,10 +711,10 @@
         <v>104.4606653849844</v>
       </c>
       <c r="C23">
-        <v>109.7569555624327</v>
+        <v>109.7565200581648</v>
       </c>
       <c r="D23">
-        <v>110.9097926836878</v>
+        <v>110.9105228351089</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -725,10 +725,10 @@
         <v>108.0037543845483</v>
       </c>
       <c r="C24">
-        <v>111.0571117875137</v>
+        <v>111.0561044033226</v>
       </c>
       <c r="D24">
-        <v>111.6037836647248</v>
+        <v>111.6042815320634</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -739,10 +739,10 @@
         <v>110.5033238992442</v>
       </c>
       <c r="C25">
-        <v>113.3715260360211</v>
+        <v>113.3729689244723</v>
       </c>
       <c r="D25">
-        <v>112.3335680749544</v>
+        <v>112.3337246122324</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -753,10 +753,10 @@
         <v>106.530947876924</v>
       </c>
       <c r="C26">
-        <v>113.4422597292104</v>
+        <v>113.4413750348544</v>
       </c>
       <c r="D26">
-        <v>113.091339820525</v>
+        <v>113.0910853602543</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -767,10 +767,10 @@
         <v>104.0901370432872</v>
       </c>
       <c r="C27">
-        <v>114.8852087527134</v>
+        <v>114.8818731511573</v>
       </c>
       <c r="D27">
-        <v>113.867714017834</v>
+        <v>113.8670235378117</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -781,10 +781,10 @@
         <v>118.588276450431</v>
       </c>
       <c r="C28">
-        <v>114.8068531158072</v>
+        <v>114.811073411711</v>
       </c>
       <c r="D28">
-        <v>114.6538820703419</v>
+        <v>114.6527985984816</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -795,10 +795,10 @@
         <v>122.0871073013163</v>
       </c>
       <c r="C29">
-        <v>115.8289276556947</v>
+        <v>115.8208094002026</v>
       </c>
       <c r="D29">
-        <v>115.445608845837</v>
+        <v>115.4441991565398</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -809,10 +809,10 @@
         <v>133.3710156747742</v>
       </c>
       <c r="C30">
-        <v>115.171506448801</v>
+        <v>115.1737453018373</v>
       </c>
       <c r="D30">
-        <v>116.2458506548638</v>
+        <v>116.2440328187347</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -823,10 +823,10 @@
         <v>124.2927477510232</v>
       </c>
       <c r="C31">
-        <v>116.0149793864551</v>
+        <v>116.0208587889027</v>
       </c>
       <c r="D31">
-        <v>117.0557778244499</v>
+        <v>117.0535707339806</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -837,10 +837,10 @@
         <v>117.0456318535268</v>
       </c>
       <c r="C32">
-        <v>117.9618356762544</v>
+        <v>117.9623513728027</v>
       </c>
       <c r="D32">
-        <v>117.8779658701665</v>
+        <v>117.8755657862392</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -851,10 +851,10 @@
         <v>116.3036079757489</v>
       </c>
       <c r="C33">
-        <v>118.9170309298341</v>
+        <v>118.9165930966985</v>
       </c>
       <c r="D33">
-        <v>118.7175972178829</v>
+        <v>118.715415563437</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -865,10 +865,10 @@
         <v>114.8024803332391</v>
       </c>
       <c r="C34">
-        <v>119.7988167818979</v>
+        <v>119.7987389184751</v>
       </c>
       <c r="D34">
-        <v>119.581191996154</v>
+        <v>119.579738791774</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -879,10 +879,10 @@
         <v>116.4775082532456</v>
       </c>
       <c r="C35">
-        <v>120.1891905061047</v>
+        <v>120.1889916479253</v>
       </c>
       <c r="D35">
-        <v>120.4684121780501</v>
+        <v>120.4682108126136</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -893,10 +893,10 @@
         <v>118.1407822940663</v>
       </c>
       <c r="C36">
-        <v>120.5557677711389</v>
+        <v>120.5551788106081</v>
       </c>
       <c r="D36">
-        <v>121.3773063050814</v>
+        <v>121.3787872155573</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -907,10 +907,10 @@
         <v>119.60317208093</v>
       </c>
       <c r="C37">
-        <v>123.7610382677583</v>
+        <v>123.7618260864565</v>
       </c>
       <c r="D37">
-        <v>122.3011804523295</v>
+        <v>122.3046052161544</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -921,10 +921,10 @@
         <v>114.7017648272237</v>
       </c>
       <c r="C38">
-        <v>122.1462841988224</v>
+        <v>122.1446120481791</v>
       </c>
       <c r="D38">
-        <v>123.2322047495388</v>
+        <v>123.2376354737851</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -935,10 +935,10 @@
         <v>112.743248286053</v>
       </c>
       <c r="C39">
-        <v>124.672155938883</v>
+        <v>124.6686722246316</v>
       </c>
       <c r="D39">
-        <v>124.1634140357301</v>
+        <v>124.170647522572</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -949,10 +949,10 @@
         <v>129.2827649894466</v>
       </c>
       <c r="C40">
-        <v>126.6874084224323</v>
+        <v>126.6925642873138</v>
       </c>
       <c r="D40">
-        <v>125.092471847686</v>
+        <v>125.1009850540946</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -963,10 +963,10 @@
         <v>133.4630831300881</v>
       </c>
       <c r="C41">
-        <v>125.5469772880352</v>
+        <v>125.531775520384</v>
       </c>
       <c r="D41">
-        <v>126.0154316732839</v>
+        <v>126.0245588493998</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -977,10 +977,10 @@
         <v>147.6079107416754</v>
       </c>
       <c r="C42">
-        <v>127.2938326898402</v>
+        <v>127.2986515903239</v>
       </c>
       <c r="D42">
-        <v>126.9305024211476</v>
+        <v>126.939579116811</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -991,10 +991,10 @@
         <v>136.1209863049451</v>
       </c>
       <c r="C43">
-        <v>128.1963743996245</v>
+        <v>128.2067572667759</v>
       </c>
       <c r="D43">
-        <v>127.8382055604871</v>
+        <v>127.8465865591697</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1005,10 +1005,10 @@
         <v>127.3875518979554</v>
       </c>
       <c r="C44">
-        <v>127.1893853226784</v>
+        <v>127.1910584769248</v>
       </c>
       <c r="D44">
-        <v>128.738577897983</v>
+        <v>128.7457909042027</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1019,10 +1019,10 @@
         <v>126.59522767863</v>
       </c>
       <c r="C45">
-        <v>129.1341896685027</v>
+        <v>129.1334567285407</v>
       </c>
       <c r="D45">
-        <v>129.6307665012663</v>
+        <v>129.636581100017</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1033,10 +1033,10 @@
         <v>123.5104632944452</v>
       </c>
       <c r="C46">
-        <v>129.6058493046388</v>
+        <v>129.6049090903379</v>
       </c>
       <c r="D46">
-        <v>130.5109301364085</v>
+        <v>130.5153830666094</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1047,10 +1047,10 @@
         <v>128.4153826610447</v>
       </c>
       <c r="C47">
-        <v>131.2797574009516</v>
+        <v>131.2807621200805</v>
       </c>
       <c r="D47">
-        <v>131.370342598031</v>
+        <v>131.3737027465596</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1061,10 +1061,10 @@
         <v>129.7350894561735</v>
       </c>
       <c r="C48">
-        <v>132.462884566781</v>
+        <v>132.4621722757429</v>
       </c>
       <c r="D48">
-        <v>132.1922704673666</v>
+        <v>132.1949671848415</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1075,10 +1075,10 @@
         <v>128.897928374986</v>
       </c>
       <c r="C49">
-        <v>134.2463025866324</v>
+        <v>134.2460101585235</v>
       </c>
       <c r="D49">
-        <v>132.9480672425077</v>
+        <v>132.9505908246251</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1089,10 +1089,10 @@
         <v>126.2268925108143</v>
       </c>
       <c r="C50">
-        <v>134.9223658892498</v>
+        <v>134.9194109443749</v>
       </c>
       <c r="D50">
-        <v>133.6054188109597</v>
+        <v>133.6081969154307</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1103,10 +1103,10 @@
         <v>122.8249045091645</v>
       </c>
       <c r="C51">
-        <v>133.8081218119373</v>
+        <v>133.8044424457916</v>
       </c>
       <c r="D51">
-        <v>134.1277849728288</v>
+        <v>134.1310640280677</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1117,10 +1117,10 @@
         <v>132.3341272874356</v>
       </c>
       <c r="C52">
-        <v>133.5037461750791</v>
+        <v>133.5103804860811</v>
       </c>
       <c r="D52">
-        <v>134.477492164624</v>
+        <v>134.4812467402243</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1131,10 +1131,10 @@
         <v>145.2804985520721</v>
       </c>
       <c r="C53">
-        <v>136.1941348622052</v>
+        <v>136.1708191612503</v>
       </c>
       <c r="D53">
-        <v>134.620596549182</v>
+        <v>134.6244951716647</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1145,10 +1145,10 @@
         <v>154.1561639128665</v>
       </c>
       <c r="C54">
-        <v>135.0745089416096</v>
+        <v>135.0831487768671</v>
       </c>
       <c r="D54">
-        <v>134.5271959475096</v>
+        <v>134.5307671326594</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1159,10 +1159,10 @@
         <v>140.5034842166976</v>
       </c>
       <c r="C55">
-        <v>132.910058939761</v>
+        <v>132.9247348054379</v>
       </c>
       <c r="D55">
-        <v>134.1775051179096</v>
+        <v>134.1804701488697</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1173,10 +1173,10 @@
         <v>136.6386880537158</v>
       </c>
       <c r="C56">
-        <v>135.4044862638615</v>
+        <v>135.4076197624908</v>
       </c>
       <c r="D56">
-        <v>133.5709969211732</v>
+        <v>133.5731416519008</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1187,10 +1187,10 @@
         <v>131.340921435527</v>
       </c>
       <c r="C57">
-        <v>135.5431110523924</v>
+        <v>135.5419784574069</v>
       </c>
       <c r="D57">
-        <v>132.7246340766827</v>
+        <v>132.725869434078</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1201,10 +1201,10 @@
         <v>132.1859384898846</v>
       </c>
       <c r="C58">
-        <v>135.6363392794121</v>
+        <v>135.6343383757467</v>
       </c>
       <c r="D58">
-        <v>131.6744362287274</v>
+        <v>131.6747996538702</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1215,10 +1215,10 @@
         <v>130.3951788425591</v>
       </c>
       <c r="C59">
-        <v>132.3970070551157</v>
+        <v>132.3989663989771</v>
       </c>
       <c r="D59">
-        <v>130.4733292129677</v>
+        <v>130.4730082132473</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1229,10 +1229,10 @@
         <v>125.5275632926216</v>
       </c>
       <c r="C60">
-        <v>129.6401181990709</v>
+        <v>129.6389913961881</v>
       </c>
       <c r="D60">
-        <v>129.1913700434419</v>
+        <v>129.1906298135981</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1243,10 +1243,10 @@
         <v>123.4660057940766</v>
       </c>
       <c r="C61">
-        <v>125.846368578792</v>
+        <v>125.8455360377929</v>
       </c>
       <c r="D61">
-        <v>127.907367499513</v>
+        <v>127.9064907587622</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1257,10 +1257,10 @@
         <v>116.7584192020652</v>
       </c>
       <c r="C62">
-        <v>124.3678688261166</v>
+        <v>124.3645989921638</v>
       </c>
       <c r="D62">
-        <v>126.7071027438308</v>
+        <v>126.7063082582487</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1271,10 +1271,10 @@
         <v>114.8588614859279</v>
       </c>
       <c r="C63">
-        <v>126.3641202274572</v>
+        <v>126.3605181143258</v>
       </c>
       <c r="D63">
-        <v>125.6737037524496</v>
+        <v>125.6731094208146</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1285,10 +1285,10 @@
         <v>126.1656026102611</v>
       </c>
       <c r="C64">
-        <v>123.6742423667017</v>
+        <v>123.6811143137662</v>
       </c>
       <c r="D64">
-        <v>124.8769083575761</v>
+        <v>124.8765321230226</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1299,10 +1299,10 @@
         <v>127.9905588745035</v>
       </c>
       <c r="C65">
-        <v>122.0750735193604</v>
+        <v>122.0479549345898</v>
       </c>
       <c r="D65">
-        <v>124.366832820737</v>
+        <v>124.3666276691589</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1313,10 +1313,10 @@
         <v>133.0356704781431</v>
       </c>
       <c r="C66">
-        <v>121.2169598564116</v>
+        <v>121.2275240519117</v>
       </c>
       <c r="D66">
-        <v>124.1730574826873</v>
+        <v>124.1728973391223</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1327,10 +1327,10 @@
         <v>129.312658048059</v>
       </c>
       <c r="C67">
-        <v>122.1596220982156</v>
+        <v>122.1761764874688</v>
       </c>
       <c r="D67">
-        <v>124.303038483768</v>
+        <v>124.3027711983059</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1341,10 +1341,10 @@
         <v>127.3630583750141</v>
       </c>
       <c r="C68">
-        <v>124.8347178049719</v>
+        <v>124.8378632331325</v>
       </c>
       <c r="D68">
-        <v>124.7439820076089</v>
+        <v>124.7434924725558</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1355,10 +1355,10 @@
         <v>124.0032862089465</v>
       </c>
       <c r="C69">
-        <v>126.3645594861256</v>
+        <v>126.3634555918467</v>
       </c>
       <c r="D69">
-        <v>125.4651658007824</v>
+        <v>125.4643603854456</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1369,10 +1369,10 @@
         <v>126.1851281247277</v>
       </c>
       <c r="C70">
-        <v>128.0277442401512</v>
+        <v>128.0257027062501</v>
       </c>
       <c r="D70">
-        <v>126.4239975038398</v>
+        <v>126.4228428446738</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1383,10 +1383,10 @@
         <v>127.0798618826952</v>
       </c>
       <c r="C71">
-        <v>128.9468415428195</v>
+        <v>128.9492036825216</v>
       </c>
       <c r="D71">
-        <v>127.5675486338529</v>
+        <v>127.5660697958891</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1397,10 +1397,10 @@
         <v>127.0921917802913</v>
       </c>
       <c r="C72">
-        <v>129.3313828145833</v>
+        <v>129.3291392362704</v>
       </c>
       <c r="D72">
-        <v>128.8391370682386</v>
+        <v>128.8374120899719</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1411,10 +1411,10 @@
         <v>126.2865638055583</v>
       </c>
       <c r="C73">
-        <v>128.768728235392</v>
+        <v>128.7686096739812</v>
       </c>
       <c r="D73">
-        <v>130.1845743544382</v>
+        <v>130.1827311735873</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1425,10 +1425,10 @@
         <v>121.5056785292316</v>
       </c>
       <c r="C74">
-        <v>131.6066307766114</v>
+        <v>131.6029679862836</v>
       </c>
       <c r="D74">
-        <v>131.5580281187125</v>
+        <v>131.5561792189021</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1439,10 +1439,10 @@
         <v>119.8228020920397</v>
       </c>
       <c r="C75">
-        <v>133.2331738746498</v>
+        <v>133.2296304889724</v>
       </c>
       <c r="D75">
-        <v>132.9179248833089</v>
+        <v>132.9161918812174</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1453,10 +1453,10 @@
         <v>136.8955016204612</v>
       </c>
       <c r="C76">
-        <v>134.4293269760129</v>
+        <v>134.4365331519959</v>
       </c>
       <c r="D76">
-        <v>134.2326770142881</v>
+        <v>134.2311925865415</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1467,10 +1467,10 @@
         <v>145.7741314930178</v>
       </c>
       <c r="C77">
-        <v>136.8752353326228</v>
+        <v>136.8458925221562</v>
       </c>
       <c r="D77">
-        <v>135.4780007085941</v>
+        <v>135.4768422300486</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1481,10 +1481,10 @@
         <v>158.1106315304388</v>
       </c>
       <c r="C78">
-        <v>139.2235460179926</v>
+        <v>139.2351284046819</v>
       </c>
       <c r="D78">
-        <v>136.6397446894804</v>
+        <v>136.6389516740284</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1495,10 +1495,10 @@
         <v>149.8615520080544</v>
       </c>
       <c r="C79">
-        <v>140.569973001725</v>
+        <v>140.5877334254786</v>
       </c>
       <c r="D79">
-        <v>137.7111594959408</v>
+        <v>137.7107989733165</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1509,10 +1509,10 @@
         <v>139.5056866287273</v>
       </c>
       <c r="C80">
-        <v>139.0238810041266</v>
+        <v>139.0267668311291</v>
       </c>
       <c r="D80">
-        <v>138.696306486123</v>
+        <v>138.6962945443745</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1523,10 +1523,10 @@
         <v>137.2459806871557</v>
       </c>
       <c r="C81">
-        <v>139.5605503798816</v>
+        <v>139.5592367290531</v>
       </c>
       <c r="D81">
-        <v>139.6102961240281</v>
+        <v>139.6105133518801</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1537,10 +1537,10 @@
         <v>136.6964267216229</v>
       </c>
       <c r="C82">
-        <v>139.5772418198063</v>
+        <v>139.5756696436069</v>
       </c>
       <c r="D82">
-        <v>140.4725280944902</v>
+        <v>140.4728463676573</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1551,10 +1551,10 @@
         <v>135.1388445069232</v>
       </c>
       <c r="C83">
-        <v>140.0315419993893</v>
+        <v>140.0339052379092</v>
       </c>
       <c r="D83">
-        <v>141.2970958607532</v>
+        <v>141.2973869236967</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1565,10 +1565,10 @@
         <v>139.5988232837222</v>
       </c>
       <c r="C84">
-        <v>142.1482578923551</v>
+        <v>142.1471169101042</v>
       </c>
       <c r="D84">
-        <v>142.0933144830439</v>
+        <v>142.0934634780133</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1579,10 +1579,10 @@
         <v>138.4776495127169</v>
       </c>
       <c r="C85">
-        <v>142.3543496954395</v>
+        <v>142.353127439144</v>
       </c>
       <c r="D85">
-        <v>142.8666251709996</v>
+        <v>142.8665488693656</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1593,10 +1593,10 @@
         <v>133.0769197185519</v>
       </c>
       <c r="C86">
-        <v>145.3777714341187</v>
+        <v>145.3744846391955</v>
       </c>
       <c r="D86">
-        <v>143.6177393167904</v>
+        <v>143.6173889520705</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1607,10 +1607,10 @@
         <v>129.5098868426219</v>
       </c>
       <c r="C87">
-        <v>144.1059928481775</v>
+        <v>144.1030335028562</v>
       </c>
       <c r="D87">
-        <v>144.338442172298</v>
+        <v>144.3378026685212</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1621,10 +1621,10 @@
         <v>147.0018390950237</v>
       </c>
       <c r="C88">
-        <v>145.2842421382701</v>
+        <v>145.2904882784866</v>
       </c>
       <c r="D88">
-        <v>145.0095525809544</v>
+        <v>145.0086457890735</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1635,10 +1635,10 @@
         <v>151.035823039618</v>
       </c>
       <c r="C89">
-        <v>144.8624610684608</v>
+        <v>144.8334048000341</v>
       </c>
       <c r="D89">
-        <v>145.6075986254424</v>
+        <v>145.6064595425727</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1649,10 +1649,10 @@
         <v>166.1783420810174</v>
       </c>
       <c r="C90">
-        <v>146.8992229774827</v>
+        <v>146.9105312181758</v>
       </c>
       <c r="D90">
-        <v>146.1091264130245</v>
+        <v>146.107861243847</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1663,10 +1663,10 @@
         <v>156.6936585122553</v>
       </c>
       <c r="C91">
-        <v>147.0100036293784</v>
+        <v>147.0277516570855</v>
       </c>
       <c r="D91">
-        <v>146.4934944588654</v>
+        <v>146.4922291403356</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1677,10 +1677,10 @@
         <v>146.3780882804684</v>
       </c>
       <c r="C92">
-        <v>146.6264068756869</v>
+        <v>146.6289591930478</v>
       </c>
       <c r="D92">
-        <v>146.74411967597</v>
+        <v>146.7429850978998</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1691,10 +1691,10 @@
         <v>146.3985053847187</v>
       </c>
       <c r="C93">
-        <v>146.7439160116589</v>
+        <v>146.742464083102</v>
       </c>
       <c r="D93">
-        <v>146.8509207024188</v>
+        <v>146.8500551618296</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1705,10 +1705,10 @@
         <v>147.170906821271</v>
       </c>
       <c r="C94">
-        <v>148.5882180105588</v>
+        <v>148.5871176217286</v>
       </c>
       <c r="D94">
-        <v>146.8111294431613</v>
+        <v>146.8106554707703</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1719,10 +1719,10 @@
         <v>145.0500024277993</v>
       </c>
       <c r="C95">
-        <v>147.1806898773179</v>
+        <v>147.1828763899383</v>
       </c>
       <c r="D95">
-        <v>146.6345938522395</v>
+        <v>146.6345686550468</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1733,10 +1733,10 @@
         <v>146.3616451241655</v>
       </c>
       <c r="C96">
-        <v>147.5950944366002</v>
+        <v>147.5944073878716</v>
       </c>
       <c r="D96">
-        <v>146.3459489620715</v>
+        <v>146.3463659659627</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1747,10 +1747,10 @@
         <v>143.3616578537433</v>
       </c>
       <c r="C97">
-        <v>147.943256039442</v>
+        <v>147.9417565755234</v>
       </c>
       <c r="D97">
-        <v>145.9804193768003</v>
+        <v>145.9812110502144</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1761,10 +1761,10 @@
         <v>136.1940812936129</v>
       </c>
       <c r="C98">
-        <v>147.2610788222247</v>
+        <v>147.2585984219445</v>
       </c>
       <c r="D98">
-        <v>145.5793320965167</v>
+        <v>145.5803841773992</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1775,10 +1775,10 @@
         <v>132.3605259407412</v>
       </c>
       <c r="C99">
-        <v>145.5209007088441</v>
+        <v>145.5198006038343</v>
       </c>
       <c r="D99">
-        <v>145.185201725022</v>
+        <v>145.1864166766828</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1789,10 +1789,10 @@
         <v>147.4410162449576</v>
       </c>
       <c r="C100">
-        <v>145.1310729017615</v>
+        <v>145.1346534070245</v>
       </c>
       <c r="D100">
-        <v>144.8408535425426</v>
+        <v>144.8421434617803</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1803,10 +1803,10 @@
         <v>145.5202783185452</v>
       </c>
       <c r="C101">
-        <v>141.2282168587656</v>
+        <v>141.2007693971264</v>
       </c>
       <c r="D101">
-        <v>144.5823521307399</v>
+        <v>144.5836409340159</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1817,10 +1817,10 @@
         <v>157.4041837193603</v>
       </c>
       <c r="C102">
-        <v>140.4654701203572</v>
+        <v>140.4768412496158</v>
       </c>
       <c r="D102">
-        <v>144.4397973055084</v>
+        <v>144.441052790592</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1831,10 +1831,10 @@
         <v>149.0331017415051</v>
       </c>
       <c r="C103">
-        <v>140.9648211932786</v>
+        <v>140.9808975256323</v>
       </c>
       <c r="D103">
-        <v>144.4338941121728</v>
+        <v>144.4350355096999</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1845,10 +1845,10 @@
         <v>146.8627996190369</v>
       </c>
       <c r="C104">
-        <v>144.4262758663851</v>
+        <v>144.4257263344096</v>
       </c>
       <c r="D104">
-        <v>144.5730114234003</v>
+        <v>144.5738612733325</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1859,10 +1859,10 @@
         <v>145.6932569888101</v>
       </c>
       <c r="C105">
-        <v>145.2005483007296</v>
+        <v>145.2021363341265</v>
       </c>
       <c r="D105">
-        <v>144.8509729906482</v>
+        <v>144.851541174852</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1873,10 +1873,10 @@
         <v>142.4715365173142</v>
       </c>
       <c r="C106">
-        <v>146.3476293483223</v>
+        <v>146.346590846872</v>
       </c>
       <c r="D106">
-        <v>145.2459102352831</v>
+        <v>145.2463105563526</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1887,10 +1887,10 @@
         <v>147.2313029553008</v>
       </c>
       <c r="C107">
-        <v>147.2937326448172</v>
+        <v>147.2948264048639</v>
       </c>
       <c r="D107">
-        <v>145.7270677344777</v>
+        <v>145.7275293775121</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1901,10 +1901,10 @@
         <v>146.3734318446863</v>
       </c>
       <c r="C108">
-        <v>147.2711390401685</v>
+        <v>147.2723619213548</v>
       </c>
       <c r="D108">
-        <v>146.2607790494027</v>
+        <v>146.2615948264</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1915,10 +1915,10 @@
         <v>143.5850580995814</v>
       </c>
       <c r="C109">
-        <v>149.0596876420003</v>
+        <v>149.0573710007383</v>
       </c>
       <c r="D109">
-        <v>146.8104994347093</v>
+        <v>146.8119619807976</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1929,10 +1929,10 @@
         <v>136.5170718250443</v>
       </c>
       <c r="C110">
-        <v>146.2220817058157</v>
+        <v>146.2199861407878</v>
       </c>
       <c r="D110">
-        <v>147.3425928313389</v>
+        <v>147.3449272568307</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1943,10 +1943,10 @@
         <v>132.795321964955</v>
       </c>
       <c r="C111">
-        <v>148.0834842470835</v>
+        <v>148.0835836814464</v>
       </c>
       <c r="D111">
-        <v>147.8287117464541</v>
+        <v>147.8320056522408</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1957,10 +1957,10 @@
         <v>149.4039456673648</v>
       </c>
       <c r="C112">
-        <v>148.5038406427012</v>
+        <v>148.5058367733363</v>
       </c>
       <c r="D112">
-        <v>148.2434517619676</v>
+        <v>148.2476231559646</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -1971,10 +1971,10 @@
         <v>155.9415958415765</v>
       </c>
       <c r="C113">
-        <v>147.7686763256947</v>
+        <v>147.7371921319404</v>
       </c>
       <c r="D113">
-        <v>148.5709427025438</v>
+        <v>148.5757898753989</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -1985,10 +1985,10 @@
         <v>167.9734791225302</v>
       </c>
       <c r="C114">
-        <v>148.8054263129239</v>
+        <v>148.8184196968571</v>
       </c>
       <c r="D114">
-        <v>148.8018882908177</v>
+        <v>148.8068571115819</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -1999,10 +1999,10 @@
         <v>156.2718644302407</v>
       </c>
       <c r="C115">
-        <v>149.4430981664753</v>
+        <v>149.4615889762663</v>
       </c>
       <c r="D115">
-        <v>148.9251992276562</v>
+        <v>148.9299657652882</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2013,10 +2013,10 @@
         <v>150.731001298259</v>
       </c>
       <c r="C116">
-        <v>148.3514872184116</v>
+        <v>148.3470449110547</v>
       </c>
       <c r="D116">
-        <v>148.9329114530266</v>
+        <v>148.9374484570742</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2027,10 +2027,10 @@
         <v>148.4214495305005</v>
       </c>
       <c r="C117">
-        <v>150.1300876192389</v>
+        <v>150.1300880062849</v>
       </c>
       <c r="D117">
-        <v>148.8203215195008</v>
+        <v>148.8249394839355</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2041,10 +2041,10 @@
         <v>147.0048441881334</v>
       </c>
       <c r="C118">
-        <v>150.3242597962993</v>
+        <v>150.3287017165788</v>
       </c>
       <c r="D118">
-        <v>148.5905517267405</v>
+        <v>148.5957447380963</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2055,10 +2055,10 @@
         <v>148.6939593959755</v>
       </c>
       <c r="C119">
-        <v>149.3590858915773</v>
+        <v>149.3624865226101</v>
       </c>
       <c r="D119">
-        <v>148.2532916300303</v>
+        <v>148.2596107627189</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2069,10 +2069,10 @@
         <v>145.69589762827</v>
       </c>
       <c r="C120">
-        <v>148.4305022463685</v>
+        <v>148.4334689545791</v>
       </c>
       <c r="D120">
-        <v>147.8209522978087</v>
+        <v>147.8285718253919</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2083,10 +2083,10 @@
         <v>142.5768791271264</v>
       </c>
       <c r="C121">
-        <v>146.6052800155361</v>
+        <v>146.5989126762621</v>
       </c>
       <c r="D121">
-        <v>147.3116460440184</v>
+        <v>147.320378577118</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2097,10 +2097,10 @@
         <v>137.9696973953764</v>
       </c>
       <c r="C122">
-        <v>146.3767884021664</v>
+        <v>146.3764302859423</v>
       </c>
       <c r="D122">
-        <v>146.7469819513319</v>
+        <v>146.7563370949103</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2111,10 +2111,10 @@
         <v>132.4863068724306</v>
       </c>
       <c r="C123">
-        <v>146.7518547580093</v>
+        <v>146.7525183701246</v>
       </c>
       <c r="D123">
-        <v>146.1540523599156</v>
+        <v>146.163320370372</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2125,10 +2125,10 @@
         <v>144.5378280834701</v>
       </c>
       <c r="C124">
-        <v>144.5809188849167</v>
+        <v>144.5806133889959</v>
       </c>
       <c r="D124">
-        <v>145.5654427865466</v>
+        <v>145.5737871544199</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2139,10 +2139,10 @@
         <v>152.3414354614714</v>
       </c>
       <c r="C125">
-        <v>144.6588984917846</v>
+        <v>144.6249023417524</v>
       </c>
       <c r="D125">
-        <v>145.0175433174291</v>
+        <v>145.0240920331774</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2153,10 +2153,10 @@
         <v>164.2032439025611</v>
       </c>
       <c r="C126">
-        <v>145.1651145109523</v>
+        <v>145.1785996596681</v>
       </c>
       <c r="D126">
-        <v>144.5464865896015</v>
+        <v>144.5505931021401</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2167,10 +2167,10 @@
         <v>153.8035240299005</v>
       </c>
       <c r="C127">
-        <v>145.0526490688197</v>
+        <v>145.0731600701058</v>
       </c>
       <c r="D127">
-        <v>144.1873092986494</v>
+        <v>144.1886994512923</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2181,10 +2181,10 @@
         <v>145.4228137340859</v>
       </c>
       <c r="C128">
-        <v>144.1862429793595</v>
+        <v>144.168307514126</v>
       </c>
       <c r="D128">
-        <v>143.9715900282303</v>
+        <v>143.9701886129978</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2195,10 +2195,10 @@
         <v>140.1053039660589</v>
       </c>
       <c r="C129">
-        <v>143.5409541698346</v>
+        <v>143.5492760563428</v>
       </c>
       <c r="D129">
-        <v>143.9254242540958</v>
+        <v>143.921333963058</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2209,10 +2209,10 @@
         <v>141.7187331995573</v>
       </c>
       <c r="C130">
-        <v>143.6159312570864</v>
+        <v>143.6255448357815</v>
       </c>
       <c r="D130">
-        <v>144.0596510917472</v>
+        <v>144.0530685740429</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2223,10 +2223,10 @@
         <v>143.3493974176129</v>
       </c>
       <c r="C131">
-        <v>144.1945490628304</v>
+        <v>144.2150529424769</v>
       </c>
       <c r="D131">
-        <v>144.3727645164887</v>
+        <v>144.3640322236458</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2237,10 +2237,10 @@
         <v>140.8775968982631</v>
       </c>
       <c r="C132">
-        <v>144.5368287019531</v>
+        <v>144.532428376455</v>
       </c>
       <c r="D132">
-        <v>144.8461643650119</v>
+        <v>144.8358885469617</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2251,10 +2251,10 @@
         <v>140.4359377491282</v>
       </c>
       <c r="C133">
-        <v>144.591088586129</v>
+        <v>144.5749850319506</v>
       </c>
       <c r="D133">
-        <v>145.4503594390806</v>
+        <v>145.4393421134469</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2265,10 +2265,10 @@
         <v>133.9981890703503</v>
       </c>
       <c r="C134">
-        <v>144.782123721199</v>
+        <v>144.780250703315</v>
       </c>
       <c r="D134">
-        <v>146.1453070507923</v>
+        <v>146.1342944368106</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2279,10 +2279,10 @@
         <v>132.627886955774</v>
       </c>
       <c r="C135">
-        <v>148.3720755905862</v>
+        <v>148.37418444355</v>
       </c>
       <c r="D135">
-        <v>146.8785519712831</v>
+        <v>146.8681008820311</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2293,10 +2293,10 @@
         <v>149.4090129833281</v>
       </c>
       <c r="C136">
-        <v>146.7956744245868</v>
+        <v>146.7954385894756</v>
       </c>
       <c r="D136">
-        <v>147.5938625068809</v>
+        <v>147.5842641126979</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2307,10 +2307,10 @@
         <v>157.4845995373143</v>
       </c>
       <c r="C137">
-        <v>148.8615273309031</v>
+        <v>148.8313349556103</v>
       </c>
       <c r="D137">
-        <v>148.2384268098097</v>
+        <v>148.2297385781834</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2321,10 +2321,10 @@
         <v>168.8861005898341</v>
       </c>
       <c r="C138">
-        <v>149.5519532139683</v>
+        <v>149.5711206934269</v>
       </c>
       <c r="D138">
-        <v>148.7648606534635</v>
+        <v>148.7570253360527</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2335,10 +2335,10 @@
         <v>162.9373900091223</v>
       </c>
       <c r="C139">
-        <v>151.9323113335348</v>
+        <v>151.9433362293354</v>
       </c>
       <c r="D139">
-        <v>149.1328073640859</v>
+        <v>149.1261071798304</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2349,10 +2349,10 @@
         <v>151.8447963430633</v>
       </c>
       <c r="C140">
-        <v>150.5947313009463</v>
+        <v>150.5662219117696</v>
       </c>
       <c r="D140">
-        <v>149.3187338639387</v>
+        <v>149.3133391169936</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2363,10 +2363,10 @@
         <v>146.4650672048623</v>
       </c>
       <c r="C141">
-        <v>149.954761879877</v>
+        <v>149.9703943329693</v>
       </c>
       <c r="D141">
-        <v>149.3168154246681</v>
+        <v>149.3130457147402</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2377,10 +2377,10 @@
         <v>145.8823237186007</v>
       </c>
       <c r="C142">
-        <v>149.2926013005589</v>
+        <v>149.30547823661</v>
       </c>
       <c r="D142">
-        <v>149.1356152478879</v>
+        <v>149.133238672385</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2391,10 +2391,10 @@
         <v>147.0458761534163</v>
       </c>
       <c r="C143">
-        <v>149.4428055619192</v>
+        <v>149.4819379118077</v>
       </c>
       <c r="D143">
-        <v>148.795890112768</v>
+        <v>148.7942855638115</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2405,10 +2405,10 @@
         <v>146.175581385648</v>
       </c>
       <c r="C144">
-        <v>148.364354068183</v>
+        <v>148.3517029716122</v>
       </c>
       <c r="D144">
-        <v>148.3314151082004</v>
+        <v>148.3296673982411</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2419,10 +2419,10 @@
         <v>141.9421187346255</v>
       </c>
       <c r="C145">
-        <v>146.7540231280814</v>
+        <v>146.7275418747306</v>
       </c>
       <c r="D145">
-        <v>147.7820500945872</v>
+        <v>147.7795652263653</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2430,13 +2430,13 @@
         <v>42370</v>
       </c>
       <c r="B146">
-        <v>134.7404747913608</v>
+        <v>134.740318289444</v>
       </c>
       <c r="C146">
-        <v>147.4949438119149</v>
+        <v>147.4891463535223</v>
       </c>
       <c r="D146">
-        <v>147.1924370642224</v>
+        <v>147.1888270272383</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2444,13 +2444,13 @@
         <v>42401</v>
       </c>
       <c r="B147">
-        <v>134.2245915684086</v>
+        <v>134.2245484934545</v>
       </c>
       <c r="C147">
-        <v>146.6250634414022</v>
+        <v>146.6221212348965</v>
       </c>
       <c r="D147">
-        <v>146.6074351198115</v>
+        <v>146.6028104881155</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2458,13 +2458,13 @@
         <v>42430</v>
       </c>
       <c r="B148">
-        <v>150.101639329048</v>
+        <v>150.101838905919</v>
       </c>
       <c r="C148">
-        <v>146.7944934372408</v>
+        <v>146.8032331021063</v>
       </c>
       <c r="D148">
-        <v>146.068977194877</v>
+        <v>146.0637619234551</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2472,13 +2472,13 @@
         <v>42461</v>
       </c>
       <c r="B149">
-        <v>153.241380594024</v>
+        <v>153.2412033641796</v>
       </c>
       <c r="C149">
-        <v>145.2677332158528</v>
+        <v>145.2598449010441</v>
       </c>
       <c r="D149">
-        <v>145.6119839021639</v>
+        <v>145.6067210287796</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2486,13 +2486,13 @@
         <v>42491</v>
       </c>
       <c r="B150">
-        <v>163.533300189347</v>
+        <v>163.5336046562773</v>
       </c>
       <c r="C150">
-        <v>144.2521296026839</v>
+        <v>144.2789586661023</v>
       </c>
       <c r="D150">
-        <v>145.2611510763243</v>
+        <v>145.2565326150792</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2500,13 +2500,13 @@
         <v>42522</v>
       </c>
       <c r="B151">
-        <v>153.6516969111608</v>
+        <v>153.6515696740751</v>
       </c>
       <c r="C151">
-        <v>144.3139811705814</v>
+        <v>144.2950404219389</v>
       </c>
       <c r="D151">
-        <v>145.0323404070786</v>
+        <v>145.0289421630991</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2514,13 +2514,13 @@
         <v>42552</v>
       </c>
       <c r="B152">
-        <v>143.7377153826797</v>
+        <v>143.7378803174986</v>
       </c>
       <c r="C152">
-        <v>144.6689804556719</v>
+        <v>144.6170075967246</v>
       </c>
       <c r="D152">
-        <v>144.9296859656176</v>
+        <v>144.9274184368081</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2528,13 +2528,13 @@
         <v>42583</v>
       </c>
       <c r="B153">
-        <v>143.671996273198</v>
+        <v>143.6719489235942</v>
       </c>
       <c r="C153">
-        <v>145.2155173557935</v>
+        <v>145.2670830461661</v>
       </c>
       <c r="D153">
-        <v>144.9496338594624</v>
+        <v>144.9486836106911</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2542,13 +2542,13 @@
         <v>42614</v>
       </c>
       <c r="B154">
-        <v>142.0032294173488</v>
+        <v>142.0031118321334</v>
       </c>
       <c r="C154">
-        <v>145.2932372565914</v>
+        <v>145.2936444251328</v>
       </c>
       <c r="D154">
-        <v>145.0834143364733</v>
+        <v>145.0852687442184</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2556,13 +2556,13 @@
         <v>42644</v>
       </c>
       <c r="B155">
-        <v>141.1325389666154</v>
+        <v>141.1324705256797</v>
       </c>
       <c r="C155">
-        <v>144.6204333231488</v>
+        <v>144.664233356107</v>
       </c>
       <c r="D155">
-        <v>145.3207126032229</v>
+        <v>145.3262840462311</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2570,13 +2570,13 @@
         <v>42675</v>
       </c>
       <c r="B156">
-        <v>144.9398570255785</v>
+        <v>144.9398458501042</v>
       </c>
       <c r="C156">
-        <v>146.0419444746379</v>
+        <v>146.0263940748668</v>
       </c>
       <c r="D156">
-        <v>145.6487858087175</v>
+        <v>145.6573998314782</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2584,13 +2584,13 @@
         <v>42705</v>
       </c>
       <c r="B157">
-        <v>142.5929331069368</v>
+        <v>142.5930127233468</v>
       </c>
       <c r="C157">
-        <v>146.9828961750906</v>
+        <v>146.9546465418696</v>
       </c>
       <c r="D157">
-        <v>146.0582144561844</v>
+        <v>146.0676823611399</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2598,13 +2598,13 @@
         <v>42736</v>
       </c>
       <c r="B158">
-        <v>136.5058443777179</v>
+        <v>136.5056417402381</v>
       </c>
       <c r="C158">
-        <v>146.8830864579195</v>
+        <v>146.85406548632</v>
       </c>
       <c r="D158">
-        <v>146.5379229148879</v>
+        <v>146.5450842111121</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2612,13 +2612,13 @@
         <v>42767</v>
       </c>
       <c r="B159">
-        <v>131.843542275363</v>
+        <v>131.8435036511555</v>
       </c>
       <c r="C159">
-        <v>146.3298826463181</v>
+        <v>146.3262613674797</v>
       </c>
       <c r="D159">
-        <v>147.0780406195329</v>
+        <v>147.079555871773</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2626,13 +2626,13 @@
         <v>42795</v>
       </c>
       <c r="B160">
-        <v>151.9468279806249</v>
+        <v>151.9470692423122</v>
       </c>
       <c r="C160">
-        <v>147.5210844266402</v>
+        <v>147.5537266770434</v>
       </c>
       <c r="D160">
-        <v>147.6679686084484</v>
+        <v>147.660998547049</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2640,13 +2640,13 @@
         <v>42826</v>
       </c>
       <c r="B161">
-        <v>153.196525163585</v>
+        <v>153.196353167718</v>
       </c>
       <c r="C161">
-        <v>147.1717259730049</v>
+        <v>147.2043675621874</v>
       </c>
       <c r="D161">
-        <v>148.2916996486631</v>
+        <v>148.2745093643623</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -2654,13 +2654,13 @@
         <v>42856</v>
       </c>
       <c r="B162">
-        <v>167.5672098508254</v>
+        <v>167.5675049406805</v>
       </c>
       <c r="C162">
-        <v>147.4859724117588</v>
+        <v>147.517381502401</v>
       </c>
       <c r="D162">
-        <v>148.9268262628203</v>
+        <v>148.8991443620855</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -2668,13 +2668,13 @@
         <v>42887</v>
       </c>
       <c r="B163">
-        <v>159.4413223709983</v>
+        <v>159.4411992770102</v>
       </c>
       <c r="C163">
-        <v>150.1366678815548</v>
+        <v>150.072617201695</v>
       </c>
       <c r="D163">
-        <v>149.5418504776672</v>
+        <v>149.5049665817754</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2682,13 +2682,13 @@
         <v>42917</v>
       </c>
       <c r="B164">
-        <v>149.9425706806799</v>
+        <v>149.9427419872084</v>
       </c>
       <c r="C164">
-        <v>150.1348605280599</v>
+        <v>150.0584124478075</v>
       </c>
       <c r="D164">
-        <v>150.1007510415084</v>
+        <v>150.0572502724926</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -2696,13 +2696,13 @@
         <v>42948</v>
       </c>
       <c r="B165">
-        <v>148.8841045787466</v>
+        <v>148.8840653071496</v>
       </c>
       <c r="C165">
-        <v>150.2950947167424</v>
+        <v>150.395934928769</v>
       </c>
       <c r="D165">
-        <v>150.5628909452863</v>
+        <v>150.5161422744018</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -2710,13 +2710,13 @@
         <v>42979</v>
       </c>
       <c r="B166">
-        <v>146.9810347120839</v>
+        <v>146.9809026771524</v>
       </c>
       <c r="C166">
-        <v>151.8720728259327</v>
+        <v>151.8476806941216</v>
       </c>
       <c r="D166">
-        <v>150.8857994335851</v>
+        <v>150.8392077663346</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -2724,13 +2724,13 @@
         <v>43009</v>
       </c>
       <c r="B167">
-        <v>148.9577125405673</v>
+        <v>148.9576293224514</v>
       </c>
       <c r="C167">
-        <v>151.525373460553</v>
+        <v>151.5490059638409</v>
       </c>
       <c r="D167">
-        <v>151.0350885587154</v>
+        <v>150.9912618816564</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -2738,13 +2738,13 @@
         <v>43040</v>
       </c>
       <c r="B168">
-        <v>151.9466344881008</v>
+        <v>151.9466165475759</v>
       </c>
       <c r="C168">
-        <v>152.6377212070104</v>
+        <v>152.6342877582784</v>
       </c>
       <c r="D168">
-        <v>150.984608737835</v>
+        <v>150.9457216201871</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -2752,13 +2752,13 @@
         <v>43070</v>
       </c>
       <c r="B169">
-        <v>146.9935456100958</v>
+        <v>146.9936467687366</v>
       </c>
       <c r="C169">
-        <v>152.2133322632003</v>
+        <v>152.193133208606</v>
       </c>
       <c r="D169">
-        <v>150.721223485853</v>
+        <v>150.6891562455195</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2766,13 +2766,13 @@
         <v>43101</v>
       </c>
       <c r="B170">
-        <v>143.0020841239074</v>
+        <v>143.0019137556669</v>
       </c>
       <c r="C170">
-        <v>152.2118906789779</v>
+        <v>152.1621989601908</v>
       </c>
       <c r="D170">
-        <v>150.2507776628398</v>
+        <v>150.2257092567207</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -2780,13 +2780,13 @@
         <v>43132</v>
       </c>
       <c r="B171">
-        <v>138.8197449410226</v>
+        <v>138.8197065069972</v>
       </c>
       <c r="C171">
-        <v>152.2058338278934</v>
+        <v>152.1967826431689</v>
       </c>
       <c r="D171">
-        <v>149.5927952862103</v>
+        <v>149.5752198607252</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -2794,13 +2794,13 @@
         <v>43160</v>
       </c>
       <c r="B172">
-        <v>155.7444493730321</v>
+        <v>155.744658175298</v>
       </c>
       <c r="C172">
-        <v>151.909073268075</v>
+        <v>151.9678161715468</v>
       </c>
       <c r="D172">
-        <v>148.7824645790138</v>
+        <v>148.7739750752662</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2808,13 +2808,13 @@
         <v>43191</v>
       </c>
       <c r="B173">
-        <v>153.299541136288</v>
+        <v>153.2994419223041</v>
       </c>
       <c r="C173">
-        <v>147.0730661815558</v>
+        <v>147.1266891182633</v>
       </c>
       <c r="D173">
-        <v>147.8640324273817</v>
+        <v>147.8680180342699</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -2822,13 +2822,13 @@
         <v>43221</v>
       </c>
       <c r="B174">
-        <v>159.6120928366543</v>
+        <v>159.6122796899062</v>
       </c>
       <c r="C174">
-        <v>143.639867765234</v>
+        <v>143.6531247247396</v>
       </c>
       <c r="D174">
-        <v>146.8881744630034</v>
+        <v>146.9085538350467</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -2836,13 +2836,13 @@
         <v>43252</v>
       </c>
       <c r="B175">
-        <v>149.0149490274899</v>
+        <v>149.0148613882218</v>
       </c>
       <c r="C175">
-        <v>142.6363279551259</v>
+        <v>142.5694480588748</v>
       </c>
       <c r="D175">
-        <v>145.9083966404886</v>
+        <v>145.9488541821854</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -2850,13 +2850,13 @@
         <v>43282</v>
       </c>
       <c r="B176">
-        <v>145.6313249380234</v>
+        <v>145.6314193161698</v>
       </c>
       <c r="C176">
-        <v>143.5197923672349</v>
+        <v>143.4151286765437</v>
       </c>
       <c r="D176">
-        <v>144.9729848181963</v>
+        <v>145.0394950049519</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -2864,13 +2864,13 @@
         <v>43313</v>
       </c>
       <c r="B177">
-        <v>146.1530598291316</v>
+        <v>146.1530002810499</v>
       </c>
       <c r="C177">
-        <v>146.2638405432994</v>
+        <v>146.417769719734</v>
       </c>
       <c r="D177">
-        <v>144.1217942322537</v>
+        <v>144.2232185485742</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -2878,13 +2878,13 @@
         <v>43344</v>
       </c>
       <c r="B178">
-        <v>137.7497591698863</v>
+        <v>137.7497243398216</v>
       </c>
       <c r="C178">
-        <v>142.9432234567125</v>
+        <v>142.8939579709302</v>
       </c>
       <c r="D178">
-        <v>143.3832936141335</v>
+        <v>143.5276920955611</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -2892,13 +2892,13 @@
         <v>43374</v>
       </c>
       <c r="B179">
-        <v>142.9652400022151</v>
+        <v>142.9653374176138</v>
       </c>
       <c r="C179">
-        <v>144.2532141612124</v>
+        <v>144.2514897018786</v>
       </c>
       <c r="D179">
-        <v>142.7770029638951</v>
+        <v>142.9647508931933</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -2906,13 +2906,13 @@
         <v>43405</v>
       </c>
       <c r="B180">
-        <v>140.9350818596134</v>
+        <v>140.9351463310657</v>
       </c>
       <c r="C180">
-        <v>141.2503054395046</v>
+        <v>141.2552589008968</v>
       </c>
       <c r="D180">
-        <v>142.3136852870613</v>
+        <v>142.5332139217726</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -2920,13 +2920,13 @@
         <v>43435</v>
       </c>
       <c r="B181">
-        <v>136.751056737791</v>
+        <v>136.7508948509399</v>
       </c>
       <c r="C181">
-        <v>141.7719497640029</v>
+        <v>141.7687207619049</v>
       </c>
       <c r="D181">
-        <v>141.9958079239347</v>
+        <v>142.2207961630548</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -2934,13 +2934,13 @@
         <v>43466</v>
       </c>
       <c r="B182">
-        <v>134.8444887192949</v>
+        <v>134.8429753471242</v>
       </c>
       <c r="C182">
-        <v>142.731223952406</v>
+        <v>142.6808547941402</v>
       </c>
       <c r="D182">
-        <v>141.8183067203425</v>
+        <v>142.0080044104691</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -2948,13 +2948,13 @@
         <v>43497</v>
       </c>
       <c r="B183">
-        <v>132.3344098633955</v>
+        <v>132.3290811702469</v>
       </c>
       <c r="C183">
-        <v>143.0244510506739</v>
+        <v>143.0212823140066</v>
       </c>
       <c r="D183">
-        <v>141.7700757564584</v>
+        <v>141.8732039874236</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -2962,13 +2962,13 @@
         <v>43525</v>
       </c>
       <c r="B184">
-        <v>144.8580710545846</v>
+        <v>144.8649131199041</v>
       </c>
       <c r="C184">
-        <v>141.3693646586358</v>
+        <v>141.4229025535296</v>
       </c>
       <c r="D184">
-        <v>141.8355080766401</v>
+        <v>141.7966522784666</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -2976,13 +2976,13 @@
         <v>43556</v>
       </c>
       <c r="B185">
-        <v>151.419146260986</v>
+        <v>151.5334862971824</v>
       </c>
       <c r="C185">
-        <v>142.053930077206</v>
+        <v>142.1767250155445</v>
       </c>
       <c r="D185">
-        <v>141.9960576424264</v>
+        <v>141.7632156847072</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -2990,13 +2990,13 @@
         <v>43586</v>
       </c>
       <c r="B186">
-        <v>163.8833665833208</v>
+        <v>163.9892727548917</v>
       </c>
       <c r="C186">
-        <v>142.0689695603504</v>
+        <v>142.1386942424601</v>
       </c>
       <c r="D186">
-        <v>142.231735416666</v>
+        <v>141.7635792139392</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3004,13 +3004,13 @@
         <v>43617</v>
       </c>
       <c r="B187">
-        <v>149.6084433371171</v>
+        <v>149.3881971293501</v>
       </c>
       <c r="C187">
-        <v>141.5658470963836</v>
+        <v>141.3733274758946</v>
       </c>
       <c r="D187">
-        <v>142.5224920668309</v>
+        <v>141.7940514618282</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3018,13 +3018,27 @@
         <v>43647</v>
       </c>
       <c r="B188">
-        <v>146.4624279864978</v>
+        <v>146.3365671478042</v>
       </c>
       <c r="C188">
-        <v>143.2431839370415</v>
+        <v>143.2420087795211</v>
       </c>
       <c r="D188">
-        <v>142.8494662870283</v>
+        <v>141.8552919687332</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="2">
+        <v>43678</v>
+      </c>
+      <c r="B189">
+        <v>140.6169496192462</v>
+      </c>
+      <c r="C189">
+        <v>141.7590035283997</v>
+      </c>
+      <c r="D189">
+        <v>141.9504092407872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>